<commit_message>
Add filter criteria for household table when filtering household_members
</commit_message>
<xml_diff>
--- a/form-files/tables/household/forms/household_new/household_new.xlsx
+++ b/form-files/tables/household/forms/household_new/household_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-10720" yWindow="300" windowWidth="23650" windowHeight="16220" activeTab="2"/>
+    <workbookView xWindow="-10720" yWindow="300" windowWidth="23650" windowHeight="16220"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>type</t>
   </si>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>household_new</t>
+  </si>
+  <si>
+    <t>household_id = ?</t>
+  </si>
+  <si>
+    <t>selectionArgs.cell_type</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>[ data('household_id') ]</t>
   </si>
 </sst>
 </file>
@@ -621,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -635,15 +647,15 @@
     <col min="4" max="4" width="51.6328125" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="31.36328125" customWidth="1"/>
-    <col min="10" max="10" width="20.81640625" customWidth="1"/>
-    <col min="11" max="11" width="27.81640625" customWidth="1"/>
-    <col min="12" max="12" width="25.36328125" customWidth="1"/>
-    <col min="13" max="13" width="29.54296875" customWidth="1"/>
+    <col min="7" max="9" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="31.36328125" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" customWidth="1"/>
+    <col min="13" max="13" width="25.36328125" customWidth="1"/>
+    <col min="14" max="14" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,22 +681,25 @@
         <v>56</v>
       </c>
       <c r="I1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -697,7 +712,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -708,7 +723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -722,7 +737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -736,7 +751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -747,7 +762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="169.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="169.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -760,23 +775,32 @@
       <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>32</v>
       </c>
-      <c r="K7" t="b">
+      <c r="L7" t="b">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="b">
+      <c r="N7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -789,7 +813,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -880,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add code to process the auxHash map when creating a new instance in the database (these are ignored when opening an existing instance).
</commit_message>
<xml_diff>
--- a/form-files/tables/household/forms/household_new/household_new.xlsx
+++ b/form-files/tables/household/forms/household_new/household_new.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>type</t>
   </si>
@@ -131,30 +131,6 @@
   </si>
   <si>
     <t>comments</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>joined_through_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> value identifies the name (elementName) in the model that should be used when scanning in the joins lists for the table_id to discover the foreign key column to filter on in the subform.
-If this is omitted, we would probably just scan the entire model to see if table_id appears anywhere and use the first match we find. </t>
-    </r>
   </si>
   <si>
     <t>values_list</t>
@@ -264,6 +240,55 @@
   </si>
   <si>
     <t>[ data('household_id') ]</t>
+  </si>
+  <si>
+    <t>auxillaryHash</t>
+  </si>
+  <si>
+    <t>auxillaryHash.cell_type</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>auxillaryHash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> defines the auxillary hash to supply when creating a new sub-form. This is an ampersand-separated list of elementName=value pairs that will be used to initialize the subform. The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>joined_through_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> value identifies the name (elementName) in the model that should be used when scanning in the joins lists for the table_id to discover the foreign key column to filter on in the subform.
+If this is omitted, we would probably just scan the entire model to see if table_id appears anywhere and use the first match we find. </t>
+    </r>
+  </si>
+  <si>
+    <t>'household_id='+escape(data('household_id'))</t>
   </si>
 </sst>
 </file>
@@ -315,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -331,6 +356,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -648,58 +676,66 @@
     <col min="5" max="5" width="38" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="9" width="20.1796875" customWidth="1"/>
-    <col min="10" max="10" width="31.36328125" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" customWidth="1"/>
-    <col min="12" max="12" width="27.81640625" customWidth="1"/>
-    <col min="13" max="13" width="25.36328125" customWidth="1"/>
-    <col min="14" max="14" width="29.54296875" customWidth="1"/>
+    <col min="10" max="10" width="27.90625" customWidth="1"/>
+    <col min="11" max="11" width="20.1796875" customWidth="1"/>
+    <col min="12" max="12" width="31.36328125" customWidth="1"/>
+    <col min="13" max="13" width="20.81640625" customWidth="1"/>
+    <col min="14" max="14" width="27.81640625" customWidth="1"/>
+    <col min="15" max="15" width="25.36328125" customWidth="1"/>
+    <col min="16" max="16" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -712,7 +748,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -723,9 +759,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -737,9 +773,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -751,7 +787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -762,9 +798,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="169.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -776,31 +812,37 @@
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="K7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
         <v>32</v>
       </c>
-      <c r="L7" t="b">
+      <c r="N7" t="b">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>1</v>
       </c>
-      <c r="N7" t="b">
+      <c r="P7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -813,7 +855,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -839,16 +881,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -917,13 +959,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -931,7 +973,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -952,10 +994,10 @@
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -989,10 +1031,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>37</v>
@@ -1012,7 +1054,7 @@
         <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Column rename 'timestamp' -> 'savepoint_timestamp' and 'saved' -> 'savepoint_type' Change 'instanceName' to 'instance_name' as data value. prelim to eliminating 'instance_name'
</commit_message>
<xml_diff>
--- a/form-files/tables/household/forms/household_new/household_new.xlsx
+++ b/form-files/tables/household/forms/household_new/household_new.xlsx
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>line_text.elementName</t>
-  </si>
-  <si>
-    <t>instanceName</t>
   </si>
   <si>
     <t xml:space="preserve">listing of subforms displays the line_text in larger font, and the line_subtext in smaller font beside an 'edit' button. </t>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>'household_id='+escape(data('household_id'))</t>
+  </si>
+  <si>
+    <t>instance_name</t>
   </si>
 </sst>
 </file>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -690,37 +690,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" t="s">
-        <v>62</v>
-      </c>
       <c r="L1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M1" t="s">
         <v>31</v>
@@ -740,10 +740,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="5"/>
@@ -761,7 +761,7 @@
     </row>
     <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="5" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -800,40 +800,40 @@
     </row>
     <row r="7" spans="1:16" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
         <v>64</v>
       </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" t="s">
-        <v>32</v>
-      </c>
       <c r="N7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" t="s">
         <v>1</v>
@@ -881,16 +881,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -959,13 +959,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -994,10 +994,10 @@
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1031,30 +1031,30 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="133.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove instance_name data value. Add an 'instance_name' setting that can specify a field in the survey. Remove obsolete prompt (stop_survey) and templates (stop_survey, repeat).
</commit_message>
<xml_diff>
--- a/form-files/tables/household/forms/household_new/household_new.xlsx
+++ b/form-files/tables/household/forms/household_new/household_new.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>type</t>
   </si>
@@ -101,21 +101,6 @@
   </si>
   <si>
     <t>household_member</t>
-  </si>
-  <si>
-    <t>line_subtext.elementName</t>
-  </si>
-  <si>
-    <t>line_subtext.isInstanceMetadata</t>
-  </si>
-  <si>
-    <t>line_text.isInstanceMetadata</t>
-  </si>
-  <si>
-    <t>line_text.elementName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">listing of subforms displays the line_text in larger font, and the line_subtext in smaller font beside an 'edit' button. </t>
   </si>
   <si>
     <t>string</t>
@@ -288,7 +273,7 @@
     <t>'household_id='+escape(data('household_id'))</t>
   </si>
   <si>
-    <t>instance_name</t>
+    <t>listing of linked forms displays the value of the field specified in the linekd form's instance_name setting field within a button. Click that button to edit that linked form.</t>
   </si>
 </sst>
 </file>
@@ -661,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -679,76 +664,60 @@
     <col min="10" max="10" width="27.90625" customWidth="1"/>
     <col min="11" max="11" width="20.1796875" customWidth="1"/>
     <col min="12" max="12" width="31.36328125" customWidth="1"/>
-    <col min="13" max="13" width="20.81640625" customWidth="1"/>
-    <col min="14" max="14" width="27.81640625" customWidth="1"/>
-    <col min="15" max="15" width="25.36328125" customWidth="1"/>
-    <col min="16" max="16" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -759,9 +728,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -773,9 +742,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -787,7 +756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -798,51 +767,39 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M7" t="s">
-        <v>64</v>
-      </c>
-      <c r="N7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -855,7 +812,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -881,16 +838,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -959,13 +916,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -973,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -994,10 +951,10 @@
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1031,30 +988,30 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="133.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed linked_table prompt to use the queries sheet, added required column query_type to queries sheet, and other validation for queries sheet in XLSXconverter
</commit_message>
<xml_diff>
--- a/form-files/tables/household/forms/household_new/household_new.xlsx
+++ b/form-files/tables/household/forms/household_new/household_new.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="240" windowWidth="23660" windowHeight="16220" activeTab="3"/>
+    <workbookView xWindow="18880" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="3" r:id="rId2"/>
     <sheet name="settings" sheetId="4" r:id="rId3"/>
     <sheet name="model" sheetId="5" r:id="rId4"/>
+    <sheet name="queries" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>type</t>
   </si>
@@ -273,12 +274,36 @@
   <si>
     <t>hideInContents</t>
   </si>
+  <si>
+    <t>query_name</t>
+  </si>
+  <si>
+    <t>query_type</t>
+  </si>
+  <si>
+    <t>uri</t>
+  </si>
+  <si>
+    <t>callback</t>
+  </si>
+  <si>
+    <t>linked_table_id</t>
+  </si>
+  <si>
+    <t>orderBy</t>
+  </si>
+  <si>
+    <t>linked_data</t>
+  </si>
+  <si>
+    <t>household_members</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -302,6 +327,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -320,10 +357,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -343,9 +391,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="12">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -644,27 +709,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="51.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="27.81640625" customWidth="1"/>
-    <col min="10" max="10" width="31.36328125" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,26 +742,14 @@
       <c r="E1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>47</v>
+      <c r="F1" t="s">
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="17.5" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -710,9 +760,8 @@
         <v>30</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -723,7 +772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -737,7 +786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -751,7 +800,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="12">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -762,33 +811,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="220.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>56</v>
       </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="12">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -799,9 +842,8 @@
         <v>17</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -821,14 +863,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -842,7 +884,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,7 +895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -864,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -875,7 +917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -904,14 +946,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>40</v>
       </c>
@@ -922,7 +964,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -930,7 +972,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="18" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -938,7 +980,7 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="18" customHeight="1">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -946,7 +988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="18" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -954,7 +996,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="18" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -969,20 +1011,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="28.36328125" customWidth="1"/>
-    <col min="5" max="5" width="45.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -999,7 +1041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="133.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="133.75" customHeight="1">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1016,13 +1058,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" ht="13.25" customHeight="1"/>
+    <row r="4" spans="1:5" ht="13.25" customHeight="1"/>
+    <row r="5" spans="1:5" ht="13.25" customHeight="1"/>
+    <row r="6" spans="1:5" ht="13.25" customHeight="1"/>
+    <row r="7" spans="1:5" ht="13.25" customHeight="1"/>
+    <row r="8" spans="1:5" ht="13.25" customHeight="1"/>
+    <row r="9" spans="1:5" ht="13.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1031,4 +1073,91 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="70.1640625" customWidth="1"/>
+    <col min="4" max="4" width="72.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="27" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Extend the functionality of selects to use linked tables for choices list
</commit_message>
<xml_diff>
--- a/form-files/tables/household/forms/household_new/household_new.xlsx
+++ b/form-files/tables/household/forms/household_new/household_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18880" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="4"/>
+    <workbookView xWindow="10040" yWindow="480" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>type</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>household_members</t>
+  </si>
+  <si>
+    <t>select_linked_data</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>Who are the two youngest members of the household?</t>
+  </si>
+  <si>
+    <t>youngest</t>
   </si>
 </sst>
 </file>
@@ -357,9 +369,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -398,17 +424,31 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -711,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -833,7 +873,10 @@
     </row>
     <row r="8" spans="1:7" ht="12">
       <c r="A8" s="4" t="s">
-        <v>3</v>
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>18</v>
@@ -844,7 +887,18 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1">
-      <c r="A9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1077,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1152,8 +1206,29 @@
         <v>55</v>
       </c>
     </row>
+    <row r="3" spans="1:10" ht="24">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>